<commit_message>
modificacion del esquema en el enum de la horario
</commit_message>
<xml_diff>
--- a/Esquema Base de Datos.xlsx
+++ b/Esquema Base de Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario iTC\Documents\Universidad\POO\Administracion-de-Empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FC00F5-CE77-41CD-9FEC-B42AAC8D874A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A036A620-5BB4-4D75-B6EF-B1C0EEC754C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2F4B2D9-7A16-4DF1-8CAC-44C759D9AF41}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="86">
   <si>
     <t>id</t>
   </si>
@@ -89,9 +89,6 @@
     <t>VAR_CHAR</t>
   </si>
   <si>
-    <t>BOOLEAN</t>
-  </si>
-  <si>
     <t>id_rol</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>horas_semanales</t>
   </si>
   <si>
-    <t>dias_laborables</t>
-  </si>
-  <si>
     <t>enum('lunes','martes','miercoles','jueves','viernes','sabado','domingo')</t>
   </si>
   <si>
@@ -276,6 +270,27 @@
   </si>
   <si>
     <t>quizas elminar este campo, puesto que en toda la tabla, cada empleado va a tender su propio contrato</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horarios_Dias_Laborables</t>
+  </si>
+  <si>
+    <t>id_horarios</t>
+  </si>
+  <si>
+    <t>id_dias_Laborables</t>
+  </si>
+  <si>
+    <t>Dias_Laborables</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>ENUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -335,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -406,11 +421,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -420,6 +457,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,8 +468,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE95E7DB-E4B8-45B6-9822-59AA5E298801}">
   <dimension ref="A3:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO10" sqref="AO10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,46 +805,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="K3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="K3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="11"/>
-      <c r="U3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="11"/>
-      <c r="AE3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="11"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="13"/>
+      <c r="U3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="13"/>
+      <c r="AE3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="13"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -816,7 +857,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>4</v>
@@ -840,7 +881,7 @@
         <v>11</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>4</v>
@@ -864,7 +905,7 @@
         <v>11</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>4</v>
@@ -888,7 +929,7 @@
         <v>11</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI4" s="7" t="s">
         <v>4</v>
@@ -908,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -930,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M5" s="2">
         <v>6</v>
@@ -952,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
@@ -974,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG5" s="2">
         <v>6</v>
@@ -995,7 +1036,7 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -1015,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>17</v>
@@ -1033,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>17</v>
@@ -1051,7 +1092,7 @@
         <v>10</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AF6" s="2" t="s">
         <v>17</v>
@@ -1071,7 +1112,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -1087,10 +1128,10 @@
         <v>10</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7" s="2">
         <v>7</v>
@@ -1103,10 +1144,10 @@
         <v>10</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W7" s="2">
         <v>25</v>
@@ -1119,10 +1160,10 @@
         <v>10</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
@@ -1135,7 +1176,7 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -1151,15 +1192,15 @@
         <v>10</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1167,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W8" s="2">
         <v>150</v>
@@ -1183,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>17</v>
@@ -1201,7 +1242,7 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -1225,10 +1266,10 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="U9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W9" s="2">
         <v>25</v>
@@ -1241,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>17</v>
@@ -1259,7 +1300,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
@@ -1283,15 +1324,15 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="U10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
@@ -1299,15 +1340,15 @@
         <v>10</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2" t="s">
@@ -1319,10 +1360,10 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1334,23 +1375,23 @@
       <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="11"/>
+      <c r="K11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="13"/>
       <c r="AD11" s="1"/>
-      <c r="AE11" s="13"/>
+      <c r="AE11" s="10"/>
       <c r="AF11" s="1"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -1375,7 +1416,7 @@
         <v>11</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>4</v>
@@ -1389,30 +1430,30 @@
       <c r="R12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U12" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="11"/>
-      <c r="AE12" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="10"/>
-      <c r="AJ12" s="10"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="11"/>
+      <c r="U12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="13"/>
+      <c r="AE12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" s="12"/>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="13"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1431,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M13" s="2">
         <v>6</v>
@@ -1459,7 +1500,7 @@
         <v>11</v>
       </c>
       <c r="X13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y13" s="7" t="s">
         <v>4</v>
@@ -1483,7 +1524,7 @@
         <v>11</v>
       </c>
       <c r="AH13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI13" s="7" t="s">
         <v>4</v>
@@ -1500,10 +1541,10 @@
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1514,7 +1555,7 @@
         <v>10</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>17</v>
@@ -1532,10 +1573,10 @@
         <v>10</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W14" s="2">
         <v>6</v>
@@ -1553,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG14" s="2">
         <v>6</v>
@@ -1571,16 +1612,16 @@
       <c r="AL14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AM14" s="12" t="s">
-        <v>80</v>
+      <c r="AM14" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1599,10 +1640,10 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="U15" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W15" s="2">
         <v>45</v>
@@ -1615,10 +1656,10 @@
         <v>10</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG15" s="2">
         <v>1</v>
@@ -1648,21 +1689,21 @@
       <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="11"/>
+      <c r="K16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="13"/>
       <c r="U16" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W16" s="2">
         <v>4</v>
@@ -1675,10 +1716,10 @@
         <v>10</v>
       </c>
       <c r="AE16" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AF16" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AG16" s="2">
         <v>10</v>
@@ -1718,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>4</v>
@@ -1733,10 +1774,10 @@
         <v>8</v>
       </c>
       <c r="U17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V17" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="V17" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="W17" s="8">
         <v>7</v>
@@ -1749,10 +1790,10 @@
         <v>10</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AF17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AG17" s="8">
         <v>7</v>
@@ -1788,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M18" s="2">
         <v>6</v>
@@ -1807,15 +1848,15 @@
         <v>10</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -1823,15 +1864,15 @@
         <v>10</v>
       </c>
       <c r="AE18" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
@@ -1859,7 +1900,7 @@
         <v>10</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>17</v>
@@ -1879,15 +1920,15 @@
         <v>10</v>
       </c>
       <c r="U19" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -1895,15 +1936,15 @@
         <v>10</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
@@ -1916,7 +1957,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -1928,33 +1969,33 @@
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="M20" s="2">
+      <c r="K20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="14">
         <v>4</v>
       </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="8" t="s">
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
+      <c r="D21" s="2">
+        <v>0</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1962,34 +2003,26 @@
       <c r="H21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="M21" s="8">
-        <v>7</v>
-      </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="16"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1999,15 +2032,15 @@
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2020,68 +2053,114 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="K24" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="13"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+      <c r="K25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="K26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
+      <c r="K27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="A28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
+      <c r="R28" s="10"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -2094,7 +2173,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>4</v>
@@ -2108,21 +2187,23 @@
       <c r="H29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+      <c r="K29" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2">
         <v>6</v>
@@ -2140,21 +2221,37 @@
       <c r="H30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
+      <c r="K30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2164,21 +2261,33 @@
       <c r="H31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
+      <c r="K31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2188,21 +2297,35 @@
       <c r="H32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
+      <c r="K32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="2"/>
@@ -2223,15 +2346,15 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2249,15 +2372,15 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2344,7 +2467,8 @@
       <c r="R42" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="K29:R29"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="U12:AB12"/>
     <mergeCell ref="AE12:AL12"/>
@@ -2354,6 +2478,7 @@
     <mergeCell ref="K11:R11"/>
     <mergeCell ref="U3:AB3"/>
     <mergeCell ref="AE3:AL3"/>
+    <mergeCell ref="K24:R24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Conexion de la base de datos con la clase empresa
</commit_message>
<xml_diff>
--- a/Esquema Base de Datos.xlsx
+++ b/Esquema Base de Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario iTC\Documents\Universidad\POO\Administracion-de-Empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A036A620-5BB4-4D75-B6EF-B1C0EEC754C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D3891B-ACA5-4F17-936C-3994575E5620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2F4B2D9-7A16-4DF1-8CAC-44C759D9AF41}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="86">
   <si>
     <t>id</t>
   </si>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE95E7DB-E4B8-45B6-9822-59AA5E298801}">
   <dimension ref="A3:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,14 +1257,22 @@
       <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="K9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="U9" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Implementacion de la actualizacion de trabajadorList, desde la base de datos
</commit_message>
<xml_diff>
--- a/Esquema Base de Datos.xlsx
+++ b/Esquema Base de Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario iTC\Documents\Universidad\POO\Administracion-de-Empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D3891B-ACA5-4F17-936C-3994575E5620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F96F51-25D3-4877-A32A-1930AB27EF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2F4B2D9-7A16-4DF1-8CAC-44C759D9AF41}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <t>foranea</t>
   </si>
   <si>
-    <t>cumpleanios</t>
-  </si>
-  <si>
     <t>BIT</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>anio_entrada</t>
   </si>
 </sst>
 </file>
@@ -459,6 +459,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,10 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE95E7DB-E4B8-45B6-9822-59AA5E298801}">
   <dimension ref="A3:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,46 +805,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="K3" s="11" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
+      <c r="K3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="U3" s="11" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="17"/>
+      <c r="U3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="13"/>
-      <c r="AE3" s="11" t="s">
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="17"/>
+      <c r="AE3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="13"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="17"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -949,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M5" s="2">
         <v>6</v>
@@ -993,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG5" s="2">
         <v>6</v>
@@ -1195,7 +1195,7 @@
         <v>38</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1261,7 +1261,7 @@
         <v>19</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1332,10 +1332,10 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="U10" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
@@ -1351,7 +1351,7 @@
         <v>50</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -1383,16 +1383,16 @@
       <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="17"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="10"/>
       <c r="AF11" s="1"/>
@@ -1438,26 +1438,26 @@
       <c r="R12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="13"/>
-      <c r="AE12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF12" s="12"/>
-      <c r="AG12" s="12"/>
-      <c r="AH12" s="12"/>
-      <c r="AI12" s="12"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="12"/>
-      <c r="AL12" s="13"/>
+      <c r="U12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="17"/>
+      <c r="AE12" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF12" s="16"/>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="16"/>
+      <c r="AI12" s="16"/>
+      <c r="AJ12" s="16"/>
+      <c r="AK12" s="16"/>
+      <c r="AL12" s="17"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1480,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M13" s="2">
         <v>6</v>
@@ -1581,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>28</v>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG14" s="2">
         <v>6</v>
@@ -1621,22 +1621,22 @@
         <v>10</v>
       </c>
       <c r="AM14" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="1"/>
@@ -1648,10 +1648,10 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="U15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W15" s="2">
         <v>45</v>
@@ -1664,10 +1664,10 @@
         <v>10</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG15" s="2">
         <v>1</v>
@@ -1697,21 +1697,21 @@
       <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="13"/>
+      <c r="K16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="17"/>
       <c r="U16" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W16" s="2">
         <v>4</v>
@@ -1724,10 +1724,10 @@
         <v>10</v>
       </c>
       <c r="AE16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF16" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="AF16" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="AG16" s="2">
         <v>10</v>
@@ -1782,10 +1782,10 @@
         <v>8</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W17" s="8">
         <v>7</v>
@@ -1798,7 +1798,7 @@
         <v>10</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AF17" s="8" t="s">
         <v>28</v>
@@ -1837,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M18" s="2">
         <v>6</v>
@@ -1856,10 +1856,10 @@
         <v>10</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
@@ -1872,10 +1872,10 @@
         <v>10</v>
       </c>
       <c r="AE18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
@@ -1908,7 +1908,7 @@
         <v>10</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>17</v>
@@ -1928,10 +1928,10 @@
         <v>10</v>
       </c>
       <c r="U19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
@@ -1944,10 +1944,10 @@
         <v>10</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
@@ -1965,7 +1965,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -1977,20 +1977,20 @@
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="15" t="s">
+      <c r="K20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M20" s="14">
+      <c r="M20" s="11">
         <v>4</v>
       </c>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="15" t="s">
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
         <v>49</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
@@ -2011,21 +2011,21 @@
       <c r="H21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="16"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="13"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2043,7 +2043,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2061,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2073,16 +2073,16 @@
       <c r="H24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K24" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="13"/>
+      <c r="K24" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="17"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="K25" s="3" t="s">
@@ -2112,10 +2112,10 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="K26" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2132,10 +2132,10 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="K27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2151,16 +2151,16 @@
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="13"/>
+      <c r="A28" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="1"/>
@@ -2195,23 +2195,23 @@
       <c r="H29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K29" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="13"/>
+      <c r="K29" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="17"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2">
         <v>6</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>37</v>
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2292,7 +2292,7 @@
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>37</v>
@@ -2306,16 +2306,16 @@
         <v>10</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="M32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>51</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>37</v>
@@ -2354,10 +2354,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2380,10 +2380,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2476,16 +2476,16 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="AE3:AL3"/>
     <mergeCell ref="K29:R29"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="U12:AB12"/>
     <mergeCell ref="AE12:AL12"/>
     <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="AE3:AL3"/>
     <mergeCell ref="K24:R24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modificacion del esquema de la base de datos
</commit_message>
<xml_diff>
--- a/Esquema Base de Datos.xlsx
+++ b/Esquema Base de Datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario iTC\Documents\Universidad\POO\Administracion-de-Empleados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario iTC\Desktop\Nueva carpeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F96F51-25D3-4877-A32A-1930AB27EF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BF7231-6EA8-48FF-A693-DD72C3463070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2F4B2D9-7A16-4DF1-8CAC-44C759D9AF41}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>correoPersonal</t>
-  </si>
-  <si>
     <t>correoEmpresarial</t>
   </si>
   <si>
@@ -291,14 +288,37 @@
   </si>
   <si>
     <t>anio_entrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trabajador</t>
+  </si>
+  <si>
+    <t>SMALLINT</t>
+  </si>
+  <si>
+    <t>id_persona</t>
+  </si>
+  <si>
+    <t>id_trabajador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -447,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -472,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE95E7DB-E4B8-45B6-9822-59AA5E298801}">
-  <dimension ref="A3:AM42"/>
+  <dimension ref="A3:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,6 +820,7 @@
     <col min="3" max="3" width="7.5546875" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
     <col min="31" max="31" width="18.33203125" customWidth="1"/>
     <col min="39" max="39" width="86.5546875" customWidth="1"/>
@@ -806,7 +828,7 @@
   <sheetData>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -816,7 +838,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="17"/>
       <c r="K3" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
@@ -826,7 +848,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="17"/>
       <c r="U3" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
@@ -836,7 +858,7 @@
       <c r="AA3" s="16"/>
       <c r="AB3" s="17"/>
       <c r="AE3" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF3" s="16"/>
       <c r="AG3" s="16"/>
@@ -857,7 +879,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>4</v>
@@ -881,7 +903,7 @@
         <v>11</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>4</v>
@@ -905,7 +927,7 @@
         <v>11</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>4</v>
@@ -929,7 +951,7 @@
         <v>11</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI4" s="7" t="s">
         <v>4</v>
@@ -949,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -971,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M5" s="2">
         <v>6</v>
@@ -993,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
@@ -1015,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG5" s="2">
         <v>6</v>
@@ -1036,30 +1058,26 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2">
-        <v>12</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M6" s="2">
         <v>25</v>
@@ -1074,10 +1092,10 @@
         <v>10</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W6" s="2">
         <v>50</v>
@@ -1092,10 +1110,10 @@
         <v>10</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AG6" s="2">
         <v>100</v>
@@ -1111,27 +1129,19 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="K7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M7" s="2">
         <v>7</v>
@@ -1144,10 +1154,10 @@
         <v>10</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W7" s="2">
         <v>25</v>
@@ -1160,10 +1170,10 @@
         <v>10</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
@@ -1175,32 +1185,24 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2">
-        <v>35</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="K8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1208,10 +1210,10 @@
         <v>10</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W8" s="2">
         <v>150</v>
@@ -1224,10 +1226,10 @@
         <v>10</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AG8" s="2">
         <v>150</v>
@@ -1241,32 +1243,26 @@
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2">
-        <v>255</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
       <c r="K9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1274,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W9" s="2">
         <v>25</v>
@@ -1290,10 +1286,10 @@
         <v>10</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AG9" s="2">
         <v>150</v>
@@ -1307,21 +1303,29 @@
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>10</v>
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1332,15 +1336,15 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="U10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
@@ -1348,15 +1352,15 @@
         <v>10</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2" t="s">
@@ -1368,23 +1372,29 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
@@ -1399,14 +1409,12 @@
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2">
-        <v>25</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1424,7 +1432,7 @@
         <v>11</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>4</v>
@@ -1439,7 +1447,7 @@
         <v>8</v>
       </c>
       <c r="U12" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
@@ -1449,7 +1457,7 @@
       <c r="AA12" s="16"/>
       <c r="AB12" s="17"/>
       <c r="AE12" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF12" s="16"/>
       <c r="AG12" s="16"/>
@@ -1461,26 +1469,24 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="2">
-        <v>12</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M13" s="2">
         <v>6</v>
@@ -1508,7 +1514,7 @@
         <v>11</v>
       </c>
       <c r="X13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y13" s="7" t="s">
         <v>4</v>
@@ -1532,7 +1538,7 @@
         <v>11</v>
       </c>
       <c r="AH13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AI13" s="7" t="s">
         <v>4</v>
@@ -1548,25 +1554,25 @@
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
+      <c r="A14" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M14" s="2">
         <v>25</v>
@@ -1581,10 +1587,10 @@
         <v>10</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W14" s="2">
         <v>6</v>
@@ -1602,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG14" s="2">
         <v>6</v>
@@ -1621,21 +1627,23 @@
         <v>10</v>
       </c>
       <c r="AM14" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="8" t="s">
         <v>10</v>
       </c>
@@ -1648,10 +1656,10 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="U15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W15" s="2">
         <v>45</v>
@@ -1664,10 +1672,10 @@
         <v>10</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG15" s="2">
         <v>1</v>
@@ -1681,24 +1689,24 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
+      <c r="A16" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2">
-        <v>30</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -1708,10 +1716,10 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="17"/>
       <c r="U16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W16" s="2">
         <v>4</v>
@@ -1724,10 +1732,10 @@
         <v>10</v>
       </c>
       <c r="AE16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF16" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="AF16" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="AG16" s="2">
         <v>10</v>
@@ -1741,22 +1749,14 @@
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2">
-        <v>30</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="K17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>11</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>4</v>
@@ -1782,10 +1782,10 @@
         <v>8</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W17" s="8">
         <v>7</v>
@@ -1798,10 +1798,10 @@
         <v>10</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AG17" s="8">
         <v>7</v>
@@ -1815,29 +1815,19 @@
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2">
-        <v>20</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="K18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M18" s="2">
         <v>6</v>
@@ -1856,15 +1846,15 @@
         <v>10</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -1872,15 +1862,15 @@
         <v>10</v>
       </c>
       <c r="AE18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
@@ -1889,37 +1879,27 @@
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
       <c r="K19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" s="2">
         <v>45</v>
       </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2" t="s">
         <v>9</v>
@@ -1927,61 +1907,53 @@
       <c r="R19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U19" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="U19" s="8"/>
+      <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
-      <c r="Y19" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE19" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF19" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="AB19" s="8"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
-      <c r="AI19" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
-      <c r="AL19" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="AL19" s="8"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>10</v>
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M20" s="11">
         <v>4</v>
@@ -1995,21 +1967,27 @@
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C21" s="2">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -2022,59 +2000,61 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C22" s="2">
+        <v>12</v>
+      </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>10</v>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C23" s="2">
+        <v>25</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>10</v>
+      <c r="H23" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C24" s="2">
+        <v>35</v>
+      </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>10</v>
+      <c r="H24" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
@@ -2085,6 +2065,22 @@
       <c r="R24" s="17"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2">
+        <v>255</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="K25" s="3" t="s">
         <v>2</v>
       </c>
@@ -2095,7 +2091,7 @@
         <v>11</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O25" s="7" t="s">
         <v>4</v>
@@ -2111,16 +2107,32 @@
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="K26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2" t="s">
@@ -2131,16 +2143,32 @@
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="K27" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
@@ -2151,16 +2179,22 @@
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="17"/>
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="1"/>
@@ -2171,32 +2205,24 @@
       <c r="R28" s="10"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>8</v>
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
@@ -2208,26 +2234,18 @@
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="2">
-        <v>6</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>10</v>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>2</v>
@@ -2239,7 +2257,7 @@
         <v>11</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O30" s="7" t="s">
         <v>4</v>
@@ -2255,25 +2273,25 @@
       </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
-        <v>10</v>
+      <c r="A31" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2291,34 +2309,20 @@
       </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="K32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="M32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="O32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" s="2" t="s">
@@ -2329,20 +2333,6 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2353,22 +2343,16 @@
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A34" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2379,21 +2363,29 @@
       <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="8" t="s">
-        <v>10</v>
+      <c r="A35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2405,6 +2397,28 @@
       <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2415,6 +2429,22 @@
       <c r="R36" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="2">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2425,6 +2455,24 @@
       <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="2">
+        <v>20</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2435,6 +2483,24 @@
       <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="2">
+        <v>18</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2445,6 +2511,22 @@
       <c r="R39" s="1"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2455,6 +2537,22 @@
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2465,6 +2563,22 @@
       <c r="R41" s="1"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2474,8 +2588,173 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M46" s="18"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A34:H34"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="K3:R3"/>
     <mergeCell ref="K11:R11"/>
@@ -2485,7 +2764,7 @@
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="U12:AB12"/>
     <mergeCell ref="AE12:AL12"/>
-    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="K24:R24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Control de ingreso y verificacion de rol
</commit_message>
<xml_diff>
--- a/Esquema Base de Datos.xlsx
+++ b/Esquema Base de Datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario iTC\Documents\Universidad\POO\Administracion-de-Empleados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i7-W11\Desktop\Administracion-de-Empleados.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F96F51-25D3-4877-A32A-1930AB27EF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D57308-C9C0-4B22-897C-161FF98AD12A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2F4B2D9-7A16-4DF1-8CAC-44C759D9AF41}"/>
   </bookViews>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -176,9 +168,6 @@
     <t>añoFundacion</t>
   </si>
   <si>
-    <t>fundador</t>
-  </si>
-  <si>
     <t>rubro</t>
   </si>
   <si>
@@ -291,6 +280,9 @@
   </si>
   <si>
     <t>anio_entrada</t>
+  </si>
+  <si>
+    <t>leyenda</t>
   </si>
 </sst>
 </file>
@@ -788,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE95E7DB-E4B8-45B6-9822-59AA5E298801}">
   <dimension ref="A3:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -971,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M5" s="2">
         <v>6</v>
@@ -993,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
@@ -1015,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG5" s="2">
         <v>6</v>
@@ -1195,12 +1187,12 @@
         <v>38</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1224,13 +1216,13 @@
         <v>10</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="AG8" s="2">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
@@ -1261,12 +1253,12 @@
         <v>19</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1290,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>17</v>
@@ -1332,15 +1324,15 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="U10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
@@ -1348,15 +1340,15 @@
         <v>10</v>
       </c>
       <c r="AE10" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2" t="s">
@@ -1439,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="U12" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
@@ -1449,7 +1441,7 @@
       <c r="AA12" s="16"/>
       <c r="AB12" s="17"/>
       <c r="AE12" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF12" s="16"/>
       <c r="AG12" s="16"/>
@@ -1480,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M13" s="2">
         <v>6</v>
@@ -1581,7 +1573,7 @@
         <v>10</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>28</v>
@@ -1602,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG14" s="2">
         <v>6</v>
@@ -1621,12 +1613,12 @@
         <v>10</v>
       </c>
       <c r="AM14" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>28</v>
@@ -1648,10 +1640,10 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="U15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W15" s="2">
         <v>45</v>
@@ -1664,10 +1656,10 @@
         <v>10</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG15" s="2">
         <v>1</v>
@@ -1698,7 +1690,7 @@
         <v>10</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -1708,10 +1700,10 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="17"/>
       <c r="U16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W16" s="2">
         <v>4</v>
@@ -1724,10 +1716,10 @@
         <v>10</v>
       </c>
       <c r="AE16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF16" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="AF16" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="AG16" s="2">
         <v>10</v>
@@ -1782,10 +1774,10 @@
         <v>8</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W17" s="8">
         <v>7</v>
@@ -1798,7 +1790,7 @@
         <v>10</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF17" s="8" t="s">
         <v>28</v>
@@ -1837,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M18" s="2">
         <v>6</v>
@@ -1856,15 +1848,15 @@
         <v>10</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -1872,15 +1864,15 @@
         <v>10</v>
       </c>
       <c r="AE18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
@@ -1908,7 +1900,7 @@
         <v>10</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>17</v>
@@ -1928,15 +1920,15 @@
         <v>10</v>
       </c>
       <c r="U19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -1944,15 +1936,15 @@
         <v>10</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
@@ -1965,7 +1957,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -1978,7 +1970,7 @@
         <v>10</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>37</v>
@@ -1996,10 +1988,10 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
@@ -2025,12 +2017,12 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -2043,12 +2035,12 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2061,12 +2053,12 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2074,7 +2066,7 @@
         <v>10</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
@@ -2112,15 +2104,15 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="K26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2" t="s">
@@ -2132,15 +2124,15 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="K27" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
@@ -2152,7 +2144,7 @@
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2196,7 +2188,7 @@
         <v>8</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
@@ -2211,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="2">
         <v>6</v>
@@ -2256,7 +2248,7 @@
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>37</v>
@@ -2273,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2292,7 +2284,7 @@
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>37</v>
@@ -2306,19 +2298,19 @@
         <v>10</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="M32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="O32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" s="2" t="s">
@@ -2330,7 +2322,7 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>37</v>
@@ -2354,15 +2346,15 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2380,15 +2372,15 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2476,17 +2468,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="AE3:AL3"/>
     <mergeCell ref="K29:R29"/>
     <mergeCell ref="K16:R16"/>
     <mergeCell ref="U12:AB12"/>
     <mergeCell ref="AE12:AL12"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="K24:R24"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="AE3:AL3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>